<commit_message>
- Future projects dynamic logc implemnetd
</commit_message>
<xml_diff>
--- a/ResourceManagement/Assets/Reports/Sample-Project-Report.xlsx
+++ b/ResourceManagement/Assets/Reports/Sample-Project-Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajen\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ResourceManagement\Assets\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC15DE0-BDD5-47C1-9422-858A9403C35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04213C72-6088-42D5-828B-38DF8808155D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{38BC7122-FDDB-46AC-9F2B-DDCAA89ACFD2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ProjectReport" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProjectReport!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProjectReport!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Project_Name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>RemainingPercentage</t>
+  </si>
+  <si>
+    <t>Project_Summary</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAB30FF-F91E-4D4D-823C-E44C61E68320}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,9 +447,10 @@
     <col min="6" max="6" width="24.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -471,12 +475,15 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{DEAB30FF-F91E-4D4D-823C-E44C61E68320}"/>
+  <autoFilter ref="A1:I1" xr:uid="{DEAB30FF-F91E-4D4D-823C-E44C61E68320}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>